<commit_message>
Fixed FutureWarning in Excel_Helper.py and updated tweets.txt
</commit_message>
<xml_diff>
--- a/Data/sentiment_lexicon.xlsx
+++ b/Data/sentiment_lexicon.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kerollos.adel\Downloads\emoji-sentiment-lexicon\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Other\Private\Master\Project\Emo-SL-Using-Text-Based-Features-and-ML-master\Emo-SL-Using-Text-Based-Features-and-ML-master\src\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACCCEF5-F44E-4D7A-8128-5685EF4DF03A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0878FADA-0BDB-41BB-91D9-034F7FD0189B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EMOJI_SENTIMENT_LEXICON" sheetId="3" r:id="rId1"/>
@@ -27,20 +27,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="196">
   <si>
     <t>سعيد</t>
   </si>
   <si>
-    <t>رائع</t>
-  </si>
-  <si>
     <t>حزين</t>
   </si>
   <si>
-    <t>قلق</t>
-  </si>
-  <si>
     <t>غاضب</t>
   </si>
   <si>
@@ -348,6 +342,279 @@
   </si>
   <si>
     <t>ܝ</t>
+  </si>
+  <si>
+    <t>🌞</t>
+  </si>
+  <si>
+    <t>🤔</t>
+  </si>
+  <si>
+    <t>🌬️</t>
+  </si>
+  <si>
+    <t>🌴</t>
+  </si>
+  <si>
+    <t>🎉</t>
+  </si>
+  <si>
+    <t>🏆</t>
+  </si>
+  <si>
+    <t>🌅</t>
+  </si>
+  <si>
+    <t>🚧</t>
+  </si>
+  <si>
+    <t>❤️</t>
+  </si>
+  <si>
+    <t>😐</t>
+  </si>
+  <si>
+    <t>🚀</t>
+  </si>
+  <si>
+    <t>📚</t>
+  </si>
+  <si>
+    <t>💪</t>
+  </si>
+  <si>
+    <t>🌈</t>
+  </si>
+  <si>
+    <t>🌧️</t>
+  </si>
+  <si>
+    <t>🔧</t>
+  </si>
+  <si>
+    <t>🤩</t>
+  </si>
+  <si>
+    <t>🌺</t>
+  </si>
+  <si>
+    <t>🏋️‍♂️</t>
+  </si>
+  <si>
+    <t>☕</t>
+  </si>
+  <si>
+    <t>🤖</t>
+  </si>
+  <si>
+    <t>😊</t>
+  </si>
+  <si>
+    <t>📖</t>
+  </si>
+  <si>
+    <t>🏃‍♂️</t>
+  </si>
+  <si>
+    <t>💼</t>
+  </si>
+  <si>
+    <t>🌠</t>
+  </si>
+  <si>
+    <t>🌳</t>
+  </si>
+  <si>
+    <t>💎</t>
+  </si>
+  <si>
+    <t>💡</t>
+  </si>
+  <si>
+    <t>🎬</t>
+  </si>
+  <si>
+    <t>🌟</t>
+  </si>
+  <si>
+    <t>🧐</t>
+  </si>
+  <si>
+    <t>💕</t>
+  </si>
+  <si>
+    <t>🌌</t>
+  </si>
+  <si>
+    <t>🛡️</t>
+  </si>
+  <si>
+    <t>🔒</t>
+  </si>
+  <si>
+    <t>👨‍👩‍👧‍👦</t>
+  </si>
+  <si>
+    <t>😮</t>
+  </si>
+  <si>
+    <t>📝</t>
+  </si>
+  <si>
+    <t>🌍</t>
+  </si>
+  <si>
+    <t>🌱</t>
+  </si>
+  <si>
+    <t>🤝</t>
+  </si>
+  <si>
+    <t>🌿</t>
+  </si>
+  <si>
+    <t>❄️</t>
+  </si>
+  <si>
+    <t>فرح</t>
+  </si>
+  <si>
+    <t>حماس</t>
+  </si>
+  <si>
+    <t>ابتسامة</t>
+  </si>
+  <si>
+    <t>سعادة</t>
+  </si>
+  <si>
+    <t>نجاح</t>
+  </si>
+  <si>
+    <t>متفائل</t>
+  </si>
+  <si>
+    <t>ممتن</t>
+  </si>
+  <si>
+    <t>فخور</t>
+  </si>
+  <si>
+    <t>مبهور</t>
+  </si>
+  <si>
+    <t>ممتع</t>
+  </si>
+  <si>
+    <t>مليء بالسعادة</t>
+  </si>
+  <si>
+    <t>مفاجآت</t>
+  </si>
+  <si>
+    <t>راحة</t>
+  </si>
+  <si>
+    <t>حب</t>
+  </si>
+  <si>
+    <t>شغف</t>
+  </si>
+  <si>
+    <t>إلهام</t>
+  </si>
+  <si>
+    <t>تشجيع</t>
+  </si>
+  <si>
+    <t>بهجة</t>
+  </si>
+  <si>
+    <t>سرور</t>
+  </si>
+  <si>
+    <t>فرحة</t>
+  </si>
+  <si>
+    <t>احتفال</t>
+  </si>
+  <si>
+    <t>انبساط</t>
+  </si>
+  <si>
+    <t>تبتهج</t>
+  </si>
+  <si>
+    <t>تألق</t>
+  </si>
+  <si>
+    <t>نشوة</t>
+  </si>
+  <si>
+    <t>سعادة غامرة</t>
+  </si>
+  <si>
+    <t>تفاؤل</t>
+  </si>
+  <si>
+    <t>انشراح</t>
+  </si>
+  <si>
+    <t>ارتياح</t>
+  </si>
+  <si>
+    <t>نغمة سعيدة</t>
+  </si>
+  <si>
+    <t>فخر</t>
+  </si>
+  <si>
+    <t>إبداع</t>
+  </si>
+  <si>
+    <t>سلام</t>
+  </si>
+  <si>
+    <t>فشل</t>
+  </si>
+  <si>
+    <t>سيء</t>
+  </si>
+  <si>
+    <t>توتر</t>
+  </si>
+  <si>
+    <t>خاب أمل</t>
+  </si>
+  <si>
+    <t>إحباط</t>
+  </si>
+  <si>
+    <t>عقبات</t>
+  </si>
+  <si>
+    <t>ملل</t>
+  </si>
+  <si>
+    <t>شاق</t>
+  </si>
+  <si>
+    <t>تعب</t>
+  </si>
+  <si>
+    <t>خذلان</t>
+  </si>
+  <si>
+    <t>فقدان</t>
+  </si>
+  <si>
+    <t>صدمة</t>
+  </si>
+  <si>
+    <t>صعب</t>
+  </si>
+  <si>
+    <t>غموض</t>
   </si>
 </sst>
 </file>
@@ -357,7 +624,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-2000401]0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,10 +641,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFCE9178"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -400,7 +676,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -408,11 +684,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,72 +977,424 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D750AA-C146-4646-85A0-40B5CC24AA72}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B3" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B4" s="5">
+        <v>-0.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B5" s="5">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="6">
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2">
-        <v>-0.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" s="6">
         <v>-0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2">
-        <v>-0.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2">
-        <v>-1</v>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="6">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B22" s="6">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" s="6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="6">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" s="6">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B30" s="6">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B31" s="6">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B32" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B33" s="6">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" s="6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B35" s="6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B36" s="6">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B37" s="6">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B38" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B39" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B40" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B41" s="6">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B42" s="6">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B43" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B44" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B45" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B46" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" s="6">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B48" s="6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B49" s="6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B50" s="6">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B51" s="6">
+        <v>-0.4</v>
       </c>
     </row>
   </sheetData>
@@ -770,24 +1405,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -795,39 +1430,399 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="2">
         <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>150</v>
       </c>
       <c r="B4" s="2">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>151</v>
       </c>
       <c r="B5" s="2">
-        <v>-0.5</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>152</v>
       </c>
       <c r="B6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="2">
         <v>-0.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B37" s="2">
+        <v>-0.9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B39" s="2">
+        <v>-0.9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B40" s="2">
+        <v>-0.7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B41" s="2">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B42" s="2">
+        <v>-0.9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B43" s="2">
+        <v>-0.7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B44" s="2">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B45" s="2">
+        <v>-0.7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B46" s="2">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B47" s="2">
+        <v>-0.9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B48" s="2">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B49" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B50" s="2">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B51" s="2">
+        <v>-0.5</v>
       </c>
     </row>
   </sheetData>
@@ -839,178 +1834,178 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{554CCFDD-441E-4989-B38D-2C37006089CF}">
   <dimension ref="A1:B87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="N86" sqref="N86"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>0</v>
       </c>
       <c r="B22" s="2">
@@ -1018,7 +2013,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>1</v>
       </c>
       <c r="B23" s="2">
@@ -1026,7 +2021,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>2</v>
       </c>
       <c r="B24" s="2">
@@ -1034,7 +2029,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>3</v>
       </c>
       <c r="B25" s="2">
@@ -1042,7 +2037,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>4</v>
       </c>
       <c r="B26" s="2">
@@ -1050,7 +2045,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <v>5</v>
       </c>
       <c r="B27" s="2">
@@ -1058,7 +2053,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="A28" s="3">
         <v>6</v>
       </c>
       <c r="B28" s="2">
@@ -1066,7 +2061,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="A29" s="3">
         <v>7</v>
       </c>
       <c r="B29" s="2">
@@ -1074,7 +2069,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="A30" s="3">
         <v>8</v>
       </c>
       <c r="B30" s="2">
@@ -1082,7 +2077,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+      <c r="A31" s="3">
         <v>9</v>
       </c>
       <c r="B31" s="2">
@@ -1091,368 +2086,368 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B32" s="2"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B34" s="2"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B35" s="2"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B36" s="2"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B37" s="2"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B38" s="2"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B39" s="2"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B40" s="2"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B41" s="2"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B42" s="2"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B43" s="2"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B44" s="2"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B45" s="2"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B46" s="2"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B47" s="2"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B48" s="2"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B49" s="2"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B50" s="2"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B54" s="2"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B56" s="2"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B57" s="2"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B58" s="2"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B59" s="2"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B60" s="2"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B61" s="2"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B62" s="2"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B63" s="2"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B64" s="2"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B65" s="2"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B66" s="2"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B67" s="2"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B68" s="2"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B69" s="2"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B70" s="2"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B71" s="2"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B72" s="2"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B73" s="2"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B74" s="2"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B75" s="2"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B76" s="2"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>